<commit_message>
Restructuring + PCR analysis
</commit_message>
<xml_diff>
--- a/data/__data_dictionary.xlsx
+++ b/data/__data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\R\Vasc-AoP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mar\Dev\Projects\R\Vasc-AoP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356894D8-0E5A-4790-99C9-BC63926316D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8BF245-DD90-4682-8C52-84C6EAA7216E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IHC" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Mouse</t>
   </si>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t>mean_segment_surface_area</t>
+  </si>
+  <si>
+    <t>P21</t>
+  </si>
+  <si>
+    <t>P70</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>21 days post-natal</t>
   </si>
 </sst>
 </file>
@@ -542,14 +554,14 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="98.28515625" customWidth="1"/>
-    <col min="3" max="3" width="99.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.53515625" customWidth="1"/>
+    <col min="2" max="2" width="98.3046875" customWidth="1"/>
+    <col min="3" max="3" width="99.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -560,7 +572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -568,7 +580,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -579,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -590,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -601,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -609,7 +621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -617,7 +629,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -625,7 +637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -633,7 +645,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -641,7 +653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -649,7 +661,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -657,7 +669,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -665,7 +677,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -673,7 +685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -681,7 +693,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -689,7 +701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -697,7 +709,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -705,7 +717,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -726,13 +738,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.15234375" customWidth="1"/>
+    <col min="2" max="2" width="38.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -743,7 +755,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -754,7 +766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -772,19 +784,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E39FA62-F62D-4A37-BD88-767EAAF3E4AB}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.3828125" customWidth="1"/>
+    <col min="3" max="3" width="10.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -795,7 +807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -806,7 +818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -817,7 +829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -826,6 +838,28 @@
       </c>
       <c r="C4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -837,18 +871,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBEE3CE-7800-4FD3-89A8-253D04570371}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.15234375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -859,7 +893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -870,7 +904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -881,7 +915,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>23</v>
       </c>

</xml_diff>